<commit_message>
feat: Implement new HTML templates for sales notes and delivery orders with embedded styles, replacing separate CSS, JS, and Excel files.
</commit_message>
<xml_diff>
--- a/invoice.xlsx
+++ b/invoice.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/941db24566e1055c/Dokumen/invoice-generator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\OneDrive\Dokumen\invoice-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FE254C5-53A5-45BC-9F9A-DE0DDFDD14CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{4FE254C5-53A5-45BC-9F9A-DE0DDFDD14CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{F71FCF11-5CD4-4F51-A5D3-0DD72C2B3B63}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9375" xr2:uid="{53A82167-C82A-427A-BE80-FBA2A7AC804B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>RAPA CEMENT &amp; GRC</t>
   </si>
@@ -93,43 +93,7 @@
     <t>Telp: 08112959125 / 082134567874</t>
   </si>
   <si>
-    <t>{{CUSTOMER_NAME}}</t>
-  </si>
-  <si>
-    <t>{{CUSTOMER_ADDRESS}}</t>
-  </si>
-  <si>
-    <t>{{PO_NUMBER}}</t>
-  </si>
-  <si>
     <t>NO. PO:</t>
-  </si>
-  <si>
-    <t>[[NO]]</t>
-  </si>
-  <si>
-    <t>[[NAME]]</t>
-  </si>
-  <si>
-    <t>[PCS]</t>
-  </si>
-  <si>
-    <t>[M2]</t>
-  </si>
-  <si>
-    <t>[PRICE]</t>
-  </si>
-  <si>
-    <t>{{SUBTOTAL}}</t>
-  </si>
-  <si>
-    <t>{{DP}}</t>
-  </si>
-  <si>
-    <t>{{ONGKIR}}</t>
-  </si>
-  <si>
-    <t>{{KEKURANGAN}}</t>
   </si>
 </sst>
 </file>
@@ -905,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F282E163-2F1F-407E-94B8-3D9BA0B90A98}">
   <dimension ref="E6:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7:Q34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,9 +952,7 @@
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
-      <c r="O10" s="5" t="s">
-        <v>22</v>
-      </c>
+      <c r="O10" s="5"/>
       <c r="P10" s="5"/>
       <c r="Q10" s="8"/>
     </row>
@@ -1007,9 +969,7 @@
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
-      <c r="O11" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="O11" s="5"/>
       <c r="P11" s="5"/>
       <c r="Q11" s="8"/>
     </row>
@@ -1048,11 +1008,9 @@
     <row r="14" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E14" s="4"/>
       <c r="F14" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>24</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
@@ -1108,26 +1066,16 @@
     </row>
     <row r="17" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E17" s="4"/>
-      <c r="F17" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="G17" s="42" t="s">
-        <v>27</v>
-      </c>
+      <c r="F17" s="24"/>
+      <c r="G17" s="42"/>
       <c r="H17" s="42"/>
       <c r="I17" s="42"/>
       <c r="J17" s="42"/>
       <c r="K17" s="42"/>
       <c r="L17" s="42"/>
-      <c r="M17" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="N17" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="O17" s="15" t="s">
-        <v>30</v>
-      </c>
+      <c r="M17" s="24"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
       <c r="P17" s="16"/>
       <c r="Q17" s="8"/>
     </row>
@@ -1265,9 +1213,7 @@
       <c r="O26" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="P26" s="19" t="s">
-        <v>31</v>
-      </c>
+      <c r="P26" s="19"/>
       <c r="Q26" s="8"/>
     </row>
     <row r="27" spans="5:17" x14ac:dyDescent="0.25">
@@ -1288,9 +1234,7 @@
       <c r="O27" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="P27" s="19" t="s">
-        <v>32</v>
-      </c>
+      <c r="P27" s="19"/>
       <c r="Q27" s="8"/>
     </row>
     <row r="28" spans="5:17" x14ac:dyDescent="0.25">
@@ -1309,9 +1253,7 @@
       <c r="O28" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="P28" s="27" t="s">
-        <v>33</v>
-      </c>
+      <c r="P28" s="27"/>
       <c r="Q28" s="8"/>
     </row>
     <row r="29" spans="5:17" x14ac:dyDescent="0.25">
@@ -1328,9 +1270,7 @@
       <c r="O29" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="P29" s="19" t="s">
-        <v>34</v>
-      </c>
+      <c r="P29" s="19"/>
       <c r="Q29" s="26"/>
     </row>
     <row r="30" spans="5:17" x14ac:dyDescent="0.25">

</xml_diff>